<commit_message>
chnaged the model run file to automatically correct the chromium values below the 0.14 threshold to 0 and the STD of these values to 1
</commit_message>
<xml_diff>
--- a/ML_PT_Pyworkflow/datasets/Unknowns-template.xlsx
+++ b/ML_PT_Pyworkflow/datasets/Unknowns-template.xlsx
@@ -2244,7 +2244,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2254,13 +2254,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2307,7 +2301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2321,14 +2315,11 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -2338,9 +2329,6 @@
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2650,50 +2638,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2818,7 +2806,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
@@ -2841,10 +2829,10 @@
         <v>3.531e-8</v>
       </c>
       <c r="H2" s="6">
-        <v>50.34455139355163</v>
+        <v>50.34</v>
       </c>
       <c r="I2" s="6">
-        <v>0.3375</v>
+        <v>0.34</v>
       </c>
       <c r="J2" s="6">
         <v>7.48</v>
@@ -2865,7 +2853,7 @@
         <v>19.49264118316946</v>
       </c>
       <c r="P2" s="6">
-        <v>0.6445</v>
+        <v>0.64</v>
       </c>
       <c r="Q2" s="6">
         <v>1.88</v>
@@ -2943,7 +2931,7 @@
         <v>0.0104</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4" t="s">
         <v>47</v>
       </c>
@@ -3068,7 +3056,7 @@
         <v>0.0101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
@@ -3193,7 +3181,7 @@
         <v>0.009899999999999999</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
@@ -3318,7 +3306,7 @@
         <v>0.0037</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4" t="s">
         <v>55</v>
       </c>
@@ -3443,7 +3431,7 @@
         <v>0.0153</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4" t="s">
         <v>58</v>
       </c>
@@ -3568,7 +3556,7 @@
         <v>0.0108</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4" t="s">
         <v>61</v>
       </c>
@@ -3693,7 +3681,7 @@
         <v>0.0111</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4" t="s">
         <v>63</v>
       </c>
@@ -3818,7 +3806,7 @@
         <v>0.011</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4" t="s">
         <v>65</v>
       </c>
@@ -3943,7 +3931,7 @@
         <v>0.018</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4" t="s">
         <v>67</v>
       </c>
@@ -4068,7 +4056,7 @@
         <v>0.0159</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4" t="s">
         <v>69</v>
       </c>
@@ -4193,7 +4181,7 @@
         <v>0.0103</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4" t="s">
         <v>72</v>
       </c>
@@ -4318,7 +4306,7 @@
         <v>0.0186</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4" t="s">
         <v>74</v>
       </c>
@@ -4443,7 +4431,7 @@
         <v>0.0178</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4" t="s">
         <v>76</v>
       </c>
@@ -4568,7 +4556,7 @@
         <v>0.0103</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4" t="s">
         <v>78</v>
       </c>
@@ -4693,7 +4681,7 @@
         <v>0.0101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4" t="s">
         <v>80</v>
       </c>
@@ -4818,7 +4806,7 @@
         <v>0.0152</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="4" t="s">
         <v>82</v>
       </c>
@@ -4943,7 +4931,7 @@
         <v>0.009000000000000001</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="4" t="s">
         <v>84</v>
       </c>
@@ -5068,7 +5056,7 @@
         <v>0.0116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4" t="s">
         <v>86</v>
       </c>
@@ -5193,7 +5181,7 @@
         <v>0.0109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4" t="s">
         <v>88</v>
       </c>
@@ -21623,7 +21611,7 @@
       <c r="R152" s="6">
         <v>100.4001202650765</v>
       </c>
-      <c r="S152" s="7"/>
+      <c r="S152" s="5"/>
       <c r="T152" s="4"/>
       <c r="U152" s="5">
         <v>10</v>
@@ -21744,7 +21732,7 @@
       <c r="R153" s="6">
         <v>99.58858463884003</v>
       </c>
-      <c r="S153" s="7"/>
+      <c r="S153" s="5"/>
       <c r="T153" s="4"/>
       <c r="U153" s="5">
         <v>11</v>
@@ -21865,7 +21853,7 @@
       <c r="R154" s="6">
         <v>99.99295995212132</v>
       </c>
-      <c r="S154" s="7"/>
+      <c r="S154" s="5"/>
       <c r="T154" s="4"/>
       <c r="U154" s="5">
         <v>12</v>
@@ -21986,7 +21974,7 @@
       <c r="R155" s="6">
         <v>99.37815178846698</v>
       </c>
-      <c r="S155" s="7"/>
+      <c r="S155" s="5"/>
       <c r="T155" s="4"/>
       <c r="U155" s="5">
         <v>13</v>
@@ -22107,7 +22095,7 @@
       <c r="R156" s="6">
         <v>99.63331626801748</v>
       </c>
-      <c r="S156" s="7"/>
+      <c r="S156" s="5"/>
       <c r="T156" s="4"/>
       <c r="U156" s="5">
         <v>14</v>
@@ -22228,7 +22216,7 @@
       <c r="R157" s="6">
         <v>99.24613623441105</v>
       </c>
-      <c r="S157" s="7"/>
+      <c r="S157" s="5"/>
       <c r="T157" s="4"/>
       <c r="U157" s="5">
         <v>15</v>
@@ -22349,7 +22337,7 @@
       <c r="R158" s="6">
         <v>100.1358992030014</v>
       </c>
-      <c r="S158" s="7"/>
+      <c r="S158" s="5"/>
       <c r="T158" s="4"/>
       <c r="U158" s="5">
         <v>16</v>
@@ -22470,7 +22458,7 @@
       <c r="R159" s="6">
         <v>100.1378394827805</v>
       </c>
-      <c r="S159" s="7"/>
+      <c r="S159" s="5"/>
       <c r="T159" s="4"/>
       <c r="U159" s="5">
         <v>40</v>
@@ -22591,7 +22579,7 @@
       <c r="R160" s="6">
         <v>99.55976644411436</v>
       </c>
-      <c r="S160" s="7"/>
+      <c r="S160" s="5"/>
       <c r="T160" s="4"/>
       <c r="U160" s="5">
         <v>41</v>
@@ -22712,7 +22700,7 @@
       <c r="R161" s="6">
         <v>100.11288252672</v>
       </c>
-      <c r="S161" s="7"/>
+      <c r="S161" s="5"/>
       <c r="T161" s="4"/>
       <c r="U161" s="5">
         <v>42</v>
@@ -22833,7 +22821,7 @@
       <c r="R162" s="6">
         <v>99.83035402146395</v>
       </c>
-      <c r="S162" s="7"/>
+      <c r="S162" s="5"/>
       <c r="T162" s="4"/>
       <c r="U162" s="5">
         <v>43</v>
@@ -22954,7 +22942,7 @@
       <c r="R163" s="6">
         <v>99.79044893647095</v>
       </c>
-      <c r="S163" s="7"/>
+      <c r="S163" s="5"/>
       <c r="T163" s="4"/>
       <c r="U163" s="5">
         <v>44</v>
@@ -23075,7 +23063,7 @@
       <c r="R164" s="6">
         <v>99.87288632239304</v>
       </c>
-      <c r="S164" s="7"/>
+      <c r="S164" s="5"/>
       <c r="T164" s="4"/>
       <c r="U164" s="5">
         <v>45</v>
@@ -23196,7 +23184,7 @@
       <c r="R165" s="6">
         <v>99.69154977442123</v>
       </c>
-      <c r="S165" s="7"/>
+      <c r="S165" s="5"/>
       <c r="T165" s="4"/>
       <c r="U165" s="5">
         <v>46</v>
@@ -23317,7 +23305,7 @@
       <c r="R166" s="6">
         <v>99.87561575907739</v>
       </c>
-      <c r="S166" s="7"/>
+      <c r="S166" s="5"/>
       <c r="T166" s="4"/>
       <c r="U166" s="5">
         <v>48</v>
@@ -23438,7 +23426,7 @@
       <c r="R167" s="6">
         <v>99.57231675060339</v>
       </c>
-      <c r="S167" s="7"/>
+      <c r="S167" s="5"/>
       <c r="T167" s="4"/>
       <c r="U167" s="5">
         <v>49</v>
@@ -23559,7 +23547,7 @@
       <c r="R168" s="6">
         <v>100.0909968318555</v>
       </c>
-      <c r="S168" s="7"/>
+      <c r="S168" s="5"/>
       <c r="T168" s="4"/>
       <c r="U168" s="5">
         <v>50</v>
@@ -23680,7 +23668,7 @@
       <c r="R169" s="6">
         <v>99.97627620478049</v>
       </c>
-      <c r="S169" s="7"/>
+      <c r="S169" s="5"/>
       <c r="T169" s="4"/>
       <c r="U169" s="5">
         <v>51</v>
@@ -23801,7 +23789,7 @@
       <c r="R170" s="6">
         <v>99.8849571972498</v>
       </c>
-      <c r="S170" s="7"/>
+      <c r="S170" s="5"/>
       <c r="T170" s="4"/>
       <c r="U170" s="5">
         <v>52</v>
@@ -23922,7 +23910,7 @@
       <c r="R171" s="6">
         <v>100.0630799597481</v>
       </c>
-      <c r="S171" s="7"/>
+      <c r="S171" s="5"/>
       <c r="T171" s="4"/>
       <c r="U171" s="5">
         <v>53</v>
@@ -24043,7 +24031,7 @@
       <c r="R172" s="6">
         <v>100.0687037054838</v>
       </c>
-      <c r="S172" s="7"/>
+      <c r="S172" s="5"/>
       <c r="T172" s="4"/>
       <c r="U172" s="5">
         <v>54</v>
@@ -24164,7 +24152,7 @@
       <c r="R173" s="6">
         <v>100.3724071074924</v>
       </c>
-      <c r="S173" s="7"/>
+      <c r="S173" s="5"/>
       <c r="T173" s="4"/>
       <c r="U173" s="5">
         <v>55</v>
@@ -24285,7 +24273,7 @@
       <c r="R174" s="6">
         <v>100.0610021651364</v>
       </c>
-      <c r="S174" s="7"/>
+      <c r="S174" s="5"/>
       <c r="T174" s="4"/>
       <c r="U174" s="5">
         <v>56</v>
@@ -24406,7 +24394,7 @@
       <c r="R175" s="6">
         <v>99.46655819111511</v>
       </c>
-      <c r="S175" s="7"/>
+      <c r="S175" s="5"/>
       <c r="T175" s="4"/>
       <c r="U175" s="5">
         <v>57</v>
@@ -24527,7 +24515,7 @@
       <c r="R176" s="6">
         <v>96.41130527588895</v>
       </c>
-      <c r="S176" s="7"/>
+      <c r="S176" s="5"/>
       <c r="T176" s="4"/>
       <c r="U176" s="5">
         <v>58</v>
@@ -24648,7 +24636,7 @@
       <c r="R177" s="6">
         <v>99.47791131948073</v>
       </c>
-      <c r="S177" s="7"/>
+      <c r="S177" s="5"/>
       <c r="T177" s="4"/>
       <c r="U177" s="5">
         <v>59</v>
@@ -24769,7 +24757,7 @@
       <c r="R178" s="6">
         <v>99.65460782346088</v>
       </c>
-      <c r="S178" s="7"/>
+      <c r="S178" s="5"/>
       <c r="T178" s="4"/>
       <c r="U178" s="5">
         <v>60</v>
@@ -24890,7 +24878,7 @@
       <c r="R179" s="6">
         <v>99.7269569017227</v>
       </c>
-      <c r="S179" s="7"/>
+      <c r="S179" s="5"/>
       <c r="T179" s="4"/>
       <c r="U179" s="5">
         <v>61</v>
@@ -25011,7 +24999,7 @@
       <c r="R180" s="6">
         <v>99.72051785578887</v>
       </c>
-      <c r="S180" s="7"/>
+      <c r="S180" s="5"/>
       <c r="T180" s="4"/>
       <c r="U180" s="5">
         <v>62</v>
@@ -25132,7 +25120,7 @@
       <c r="R181" s="6">
         <v>99.5979130142698</v>
       </c>
-      <c r="S181" s="7"/>
+      <c r="S181" s="5"/>
       <c r="T181" s="4"/>
       <c r="U181" s="5">
         <v>63</v>
@@ -25253,7 +25241,7 @@
       <c r="R182" s="6">
         <v>99.5014237819089</v>
       </c>
-      <c r="S182" s="7"/>
+      <c r="S182" s="5"/>
       <c r="T182" s="4"/>
       <c r="U182" s="5">
         <v>65</v>
@@ -25374,7 +25362,7 @@
       <c r="R183" s="6">
         <v>99.35129552574791</v>
       </c>
-      <c r="S183" s="7"/>
+      <c r="S183" s="5"/>
       <c r="T183" s="4"/>
       <c r="U183" s="5">
         <v>66</v>
@@ -25495,7 +25483,7 @@
       <c r="R184" s="6">
         <v>99.54506118967913</v>
       </c>
-      <c r="S184" s="7"/>
+      <c r="S184" s="5"/>
       <c r="T184" s="4"/>
       <c r="U184" s="5">
         <v>67</v>
@@ -25616,7 +25604,7 @@
       <c r="R185" s="6">
         <v>99.50618524116727</v>
       </c>
-      <c r="S185" s="7"/>
+      <c r="S185" s="5"/>
       <c r="T185" s="4"/>
       <c r="U185" s="5">
         <v>68</v>
@@ -25737,7 +25725,7 @@
       <c r="R186" s="6">
         <v>99.74591097246247</v>
       </c>
-      <c r="S186" s="7"/>
+      <c r="S186" s="5"/>
       <c r="T186" s="4"/>
       <c r="U186" s="5">
         <v>69</v>
@@ -25858,7 +25846,7 @@
       <c r="R187" s="6">
         <v>98.8293043479937</v>
       </c>
-      <c r="S187" s="7"/>
+      <c r="S187" s="5"/>
       <c r="T187" s="4"/>
       <c r="U187" s="5">
         <v>70</v>
@@ -25979,7 +25967,7 @@
       <c r="R188" s="6">
         <v>100.633343704098</v>
       </c>
-      <c r="S188" s="7"/>
+      <c r="S188" s="5"/>
       <c r="T188" s="4"/>
       <c r="U188" s="5">
         <v>71</v>
@@ -26100,7 +26088,7 @@
       <c r="R189" s="6">
         <v>99.804888206826</v>
       </c>
-      <c r="S189" s="7"/>
+      <c r="S189" s="5"/>
       <c r="T189" s="4"/>
       <c r="U189" s="5">
         <v>72</v>
@@ -26221,7 +26209,7 @@
       <c r="R190" s="6">
         <v>101.1517369507992</v>
       </c>
-      <c r="S190" s="7"/>
+      <c r="S190" s="5"/>
       <c r="T190" s="4"/>
       <c r="U190" s="5">
         <v>73</v>
@@ -26342,7 +26330,7 @@
       <c r="R191" s="6">
         <v>99.92866728299656</v>
       </c>
-      <c r="S191" s="7"/>
+      <c r="S191" s="5"/>
       <c r="T191" s="4"/>
       <c r="U191" s="5">
         <v>74</v>
@@ -26463,7 +26451,7 @@
       <c r="R192" s="6">
         <v>99.47345598738677</v>
       </c>
-      <c r="S192" s="7"/>
+      <c r="S192" s="5"/>
       <c r="T192" s="4"/>
       <c r="U192" s="5">
         <v>75</v>
@@ -26584,7 +26572,7 @@
       <c r="R193" s="6">
         <v>100.1422735870944</v>
       </c>
-      <c r="S193" s="7"/>
+      <c r="S193" s="5"/>
       <c r="T193" s="4"/>
       <c r="U193" s="5">
         <v>76</v>
@@ -26705,7 +26693,7 @@
       <c r="R194" s="6">
         <v>99.68939905566509</v>
       </c>
-      <c r="S194" s="7"/>
+      <c r="S194" s="5"/>
       <c r="T194" s="4"/>
       <c r="U194" s="5">
         <v>77</v>
@@ -26826,7 +26814,7 @@
       <c r="R195" s="6">
         <v>100.6737323470031</v>
       </c>
-      <c r="S195" s="7"/>
+      <c r="S195" s="5"/>
       <c r="T195" s="4"/>
       <c r="U195" s="5">
         <v>78</v>
@@ -26947,7 +26935,7 @@
       <c r="R196" s="6">
         <v>99.76278914211048</v>
       </c>
-      <c r="S196" s="7"/>
+      <c r="S196" s="5"/>
       <c r="T196" s="4"/>
       <c r="U196" s="5">
         <v>79</v>
@@ -27068,7 +27056,7 @@
       <c r="R197" s="6">
         <v>99.85584747376693</v>
       </c>
-      <c r="S197" s="7"/>
+      <c r="S197" s="5"/>
       <c r="T197" s="4"/>
       <c r="U197" s="5">
         <v>80</v>
@@ -27189,7 +27177,7 @@
       <c r="R198" s="6">
         <v>99.42911145172158</v>
       </c>
-      <c r="S198" s="7"/>
+      <c r="S198" s="5"/>
       <c r="T198" s="4"/>
       <c r="U198" s="5">
         <v>81</v>
@@ -27310,7 +27298,7 @@
       <c r="R199" s="6">
         <v>99.64477929701685</v>
       </c>
-      <c r="S199" s="7"/>
+      <c r="S199" s="5"/>
       <c r="T199" s="4"/>
       <c r="U199" s="5">
         <v>82</v>
@@ -27431,7 +27419,7 @@
       <c r="R200" s="6">
         <v>99.40612723712265</v>
       </c>
-      <c r="S200" s="7"/>
+      <c r="S200" s="5"/>
       <c r="T200" s="4"/>
       <c r="U200" s="5">
         <v>83</v>
@@ -27552,7 +27540,7 @@
       <c r="R201" s="6">
         <v>99.47573942318094</v>
       </c>
-      <c r="S201" s="7"/>
+      <c r="S201" s="5"/>
       <c r="T201" s="4"/>
       <c r="U201" s="5">
         <v>84</v>
@@ -27673,7 +27661,7 @@
       <c r="R202" s="6">
         <v>99.67220207461706</v>
       </c>
-      <c r="S202" s="7"/>
+      <c r="S202" s="5"/>
       <c r="T202" s="4"/>
       <c r="U202" s="5">
         <v>85</v>
@@ -27794,7 +27782,7 @@
       <c r="R203" s="6">
         <v>99.7405763747626</v>
       </c>
-      <c r="S203" s="7"/>
+      <c r="S203" s="5"/>
       <c r="T203" s="4"/>
       <c r="U203" s="5">
         <v>17</v>
@@ -27915,7 +27903,7 @@
       <c r="R204" s="6">
         <v>99.58312070912116</v>
       </c>
-      <c r="S204" s="7"/>
+      <c r="S204" s="5"/>
       <c r="T204" s="4"/>
       <c r="U204" s="5">
         <v>18</v>
@@ -28036,7 +28024,7 @@
       <c r="R205" s="6">
         <v>99.16185133511277</v>
       </c>
-      <c r="S205" s="7"/>
+      <c r="S205" s="5"/>
       <c r="T205" s="4"/>
       <c r="U205" s="5">
         <v>19</v>
@@ -28157,7 +28145,7 @@
       <c r="R206" s="6">
         <v>99.45241128264728</v>
       </c>
-      <c r="S206" s="7"/>
+      <c r="S206" s="5"/>
       <c r="T206" s="4"/>
       <c r="U206" s="5">
         <v>20</v>
@@ -28278,7 +28266,7 @@
       <c r="R207" s="6">
         <v>99.7235014199285</v>
       </c>
-      <c r="S207" s="7"/>
+      <c r="S207" s="5"/>
       <c r="T207" s="4"/>
       <c r="U207" s="5">
         <v>21</v>
@@ -28399,7 +28387,7 @@
       <c r="R208" s="6">
         <v>99.90679510975289</v>
       </c>
-      <c r="S208" s="7"/>
+      <c r="S208" s="5"/>
       <c r="T208" s="4"/>
       <c r="U208" s="5">
         <v>22</v>
@@ -28520,7 +28508,7 @@
       <c r="R209" s="6">
         <v>97.09730710609624</v>
       </c>
-      <c r="S209" s="7"/>
+      <c r="S209" s="5"/>
       <c r="T209" s="4"/>
       <c r="U209" s="5">
         <v>97</v>
@@ -28641,7 +28629,7 @@
       <c r="R210" s="6">
         <v>100.0680552683433</v>
       </c>
-      <c r="S210" s="7"/>
+      <c r="S210" s="5"/>
       <c r="T210" s="4"/>
       <c r="U210" s="5">
         <v>98</v>
@@ -28762,7 +28750,7 @@
       <c r="R211" s="6">
         <v>99.34478879218106</v>
       </c>
-      <c r="S211" s="7"/>
+      <c r="S211" s="5"/>
       <c r="T211" s="4"/>
       <c r="U211" s="5">
         <v>99</v>
@@ -28883,7 +28871,7 @@
       <c r="R212" s="6">
         <v>99.75826765524205</v>
       </c>
-      <c r="S212" s="7"/>
+      <c r="S212" s="5"/>
       <c r="T212" s="4"/>
       <c r="U212" s="5">
         <v>100</v>
@@ -29004,7 +28992,7 @@
       <c r="R213" s="6">
         <v>99.96314510661188</v>
       </c>
-      <c r="S213" s="7"/>
+      <c r="S213" s="5"/>
       <c r="T213" s="4"/>
       <c r="U213" s="5">
         <v>101</v>
@@ -29125,7 +29113,7 @@
       <c r="R214" s="6">
         <v>100.299712320959</v>
       </c>
-      <c r="S214" s="7"/>
+      <c r="S214" s="5"/>
       <c r="T214" s="4"/>
       <c r="U214" s="5">
         <v>102</v>
@@ -29246,7 +29234,7 @@
       <c r="R215" s="6">
         <v>99.8321674068752</v>
       </c>
-      <c r="S215" s="7"/>
+      <c r="S215" s="5"/>
       <c r="T215" s="4"/>
       <c r="U215" s="5">
         <v>103</v>
@@ -29367,7 +29355,7 @@
       <c r="R216" s="6">
         <v>99.61495978651487</v>
       </c>
-      <c r="S216" s="7"/>
+      <c r="S216" s="5"/>
       <c r="T216" s="4"/>
       <c r="U216" s="5">
         <v>104</v>
@@ -29488,7 +29476,7 @@
       <c r="R217" s="6">
         <v>99.38749925110488</v>
       </c>
-      <c r="S217" s="7"/>
+      <c r="S217" s="5"/>
       <c r="T217" s="4"/>
       <c r="U217" s="5">
         <v>105</v>
@@ -29609,7 +29597,7 @@
       <c r="R218" s="6">
         <v>99.56557435941166</v>
       </c>
-      <c r="S218" s="7"/>
+      <c r="S218" s="5"/>
       <c r="T218" s="4"/>
       <c r="U218" s="5">
         <v>106</v>
@@ -29730,7 +29718,7 @@
       <c r="R219" s="6">
         <v>99.84173838427738</v>
       </c>
-      <c r="S219" s="7"/>
+      <c r="S219" s="5"/>
       <c r="T219" s="4"/>
       <c r="U219" s="5">
         <v>107</v>
@@ -29851,7 +29839,7 @@
       <c r="R220" s="6">
         <v>96.92364282490327</v>
       </c>
-      <c r="S220" s="7"/>
+      <c r="S220" s="5"/>
       <c r="T220" s="4"/>
       <c r="U220" s="5">
         <v>108</v>
@@ -29972,7 +29960,7 @@
       <c r="R221" s="6">
         <v>99.67159485495411</v>
       </c>
-      <c r="S221" s="7"/>
+      <c r="S221" s="5"/>
       <c r="T221" s="4"/>
       <c r="U221" s="5">
         <v>109</v>
@@ -30093,7 +30081,7 @@
       <c r="R222" s="6">
         <v>99.67252822463914</v>
       </c>
-      <c r="S222" s="7"/>
+      <c r="S222" s="5"/>
       <c r="T222" s="4"/>
       <c r="U222" s="5">
         <v>110</v>
@@ -30214,7 +30202,7 @@
       <c r="R223" s="6">
         <v>99.33104960508494</v>
       </c>
-      <c r="S223" s="7"/>
+      <c r="S223" s="5"/>
       <c r="T223" s="4"/>
       <c r="U223" s="5">
         <v>111</v>
@@ -30335,7 +30323,7 @@
       <c r="R224" s="6">
         <v>99.68796873005927</v>
       </c>
-      <c r="S224" s="7"/>
+      <c r="S224" s="5"/>
       <c r="T224" s="4"/>
       <c r="U224" s="5">
         <v>112</v>
@@ -30456,7 +30444,7 @@
       <c r="R225" s="6">
         <v>100.055899797306</v>
       </c>
-      <c r="S225" s="7"/>
+      <c r="S225" s="5"/>
       <c r="T225" s="4"/>
       <c r="U225" s="5">
         <v>113</v>
@@ -30577,7 +30565,7 @@
       <c r="R226" s="6">
         <v>99.75996309770518</v>
       </c>
-      <c r="S226" s="7"/>
+      <c r="S226" s="5"/>
       <c r="T226" s="4"/>
       <c r="U226" s="5">
         <v>114</v>
@@ -30698,7 +30686,7 @@
       <c r="R227" s="6">
         <v>99.79761466693286</v>
       </c>
-      <c r="S227" s="7"/>
+      <c r="S227" s="5"/>
       <c r="T227" s="4"/>
       <c r="U227" s="5">
         <v>115</v>
@@ -30819,7 +30807,7 @@
       <c r="R228" s="6">
         <v>99.60436505854291</v>
       </c>
-      <c r="S228" s="7"/>
+      <c r="S228" s="5"/>
       <c r="T228" s="4"/>
       <c r="U228" s="5">
         <v>116</v>
@@ -30940,7 +30928,7 @@
       <c r="R229" s="6">
         <v>99.92054921790098</v>
       </c>
-      <c r="S229" s="7"/>
+      <c r="S229" s="5"/>
       <c r="T229" s="4"/>
       <c r="U229" s="5">
         <v>23</v>
@@ -31061,7 +31049,7 @@
       <c r="R230" s="6">
         <v>99.94135223663949</v>
       </c>
-      <c r="S230" s="7"/>
+      <c r="S230" s="5"/>
       <c r="T230" s="4"/>
       <c r="U230" s="5">
         <v>24</v>
@@ -31182,7 +31170,7 @@
       <c r="R231" s="6">
         <v>99.31430415593108</v>
       </c>
-      <c r="S231" s="7"/>
+      <c r="S231" s="5"/>
       <c r="T231" s="4"/>
       <c r="U231" s="5">
         <v>25</v>
@@ -31303,7 +31291,7 @@
       <c r="R232" s="6">
         <v>99.75671641675565</v>
       </c>
-      <c r="S232" s="7"/>
+      <c r="S232" s="5"/>
       <c r="T232" s="4"/>
       <c r="U232" s="5">
         <v>26</v>
@@ -31424,7 +31412,7 @@
       <c r="R233" s="6">
         <v>99.3650570928161</v>
       </c>
-      <c r="S233" s="7"/>
+      <c r="S233" s="5"/>
       <c r="T233" s="4"/>
       <c r="U233" s="5">
         <v>27</v>
@@ -31545,7 +31533,7 @@
       <c r="R234" s="6">
         <v>99.48534580523317</v>
       </c>
-      <c r="S234" s="7"/>
+      <c r="S234" s="5"/>
       <c r="T234" s="4"/>
       <c r="U234" s="5">
         <v>28</v>
@@ -31666,7 +31654,7 @@
       <c r="R235" s="6">
         <v>99.63540409323171</v>
       </c>
-      <c r="S235" s="7"/>
+      <c r="S235" s="5"/>
       <c r="T235" s="4"/>
       <c r="U235" s="5">
         <v>29</v>
@@ -31787,7 +31775,7 @@
       <c r="R236" s="6">
         <v>99.50391223686606</v>
       </c>
-      <c r="S236" s="7"/>
+      <c r="S236" s="5"/>
       <c r="T236" s="4"/>
       <c r="U236" s="5">
         <v>30</v>
@@ -31908,7 +31896,7 @@
       <c r="R237" s="6">
         <v>99.72319022014324</v>
       </c>
-      <c r="S237" s="7"/>
+      <c r="S237" s="5"/>
       <c r="T237" s="4"/>
       <c r="U237" s="5">
         <v>31</v>
@@ -32029,7 +32017,7 @@
       <c r="R238" s="6">
         <v>100.7240295861633</v>
       </c>
-      <c r="S238" s="7"/>
+      <c r="S238" s="5"/>
       <c r="T238" s="4"/>
       <c r="U238" s="5">
         <v>32</v>
@@ -32150,7 +32138,7 @@
       <c r="R239" s="6">
         <v>96.52842452350458</v>
       </c>
-      <c r="S239" s="7"/>
+      <c r="S239" s="5"/>
       <c r="T239" s="4"/>
       <c r="U239" s="5">
         <v>33</v>
@@ -32271,7 +32259,7 @@
       <c r="R240" s="6">
         <v>99.94758238383523</v>
       </c>
-      <c r="S240" s="7"/>
+      <c r="S240" s="5"/>
       <c r="T240" s="4"/>
       <c r="U240" s="5">
         <v>34</v>
@@ -32392,7 +32380,7 @@
       <c r="R241" s="6">
         <v>99.64040354156941</v>
       </c>
-      <c r="S241" s="7"/>
+      <c r="S241" s="5"/>
       <c r="T241" s="4"/>
       <c r="U241" s="5">
         <v>35</v>
@@ -32513,7 +32501,7 @@
       <c r="R242" s="6">
         <v>99.30212750951232</v>
       </c>
-      <c r="S242" s="7"/>
+      <c r="S242" s="5"/>
       <c r="T242" s="4"/>
       <c r="U242" s="5">
         <v>36</v>
@@ -32634,7 +32622,7 @@
       <c r="R243" s="6">
         <v>99.25675186285015</v>
       </c>
-      <c r="S243" s="7"/>
+      <c r="S243" s="5"/>
       <c r="T243" s="4"/>
       <c r="U243" s="5">
         <v>37</v>
@@ -32755,7 +32743,7 @@
       <c r="R244" s="6">
         <v>99.62585910720277</v>
       </c>
-      <c r="S244" s="7"/>
+      <c r="S244" s="5"/>
       <c r="T244" s="4"/>
       <c r="U244" s="5">
         <v>38</v>
@@ -32876,7 +32864,7 @@
       <c r="R245" s="6">
         <v>99.83738786113281</v>
       </c>
-      <c r="S245" s="7"/>
+      <c r="S245" s="5"/>
       <c r="T245" s="4"/>
       <c r="U245" s="5">
         <v>39</v>
@@ -32997,7 +32985,7 @@
       <c r="R246" s="6">
         <v>100.441044359726</v>
       </c>
-      <c r="S246" s="7"/>
+      <c r="S246" s="5"/>
       <c r="T246" s="4"/>
       <c r="U246" s="5">
         <v>86</v>
@@ -33118,7 +33106,7 @@
       <c r="R247" s="6">
         <v>99.92630931622902</v>
       </c>
-      <c r="S247" s="7"/>
+      <c r="S247" s="5"/>
       <c r="T247" s="4"/>
       <c r="U247" s="5">
         <v>95</v>
@@ -33239,7 +33227,7 @@
       <c r="R248" s="6">
         <v>99.18467491224648</v>
       </c>
-      <c r="S248" s="7"/>
+      <c r="S248" s="5"/>
       <c r="T248" s="4"/>
       <c r="U248" s="5">
         <v>96</v>
@@ -33360,7 +33348,7 @@
       <c r="R249" s="6">
         <v>99.86487718216047</v>
       </c>
-      <c r="S249" s="7"/>
+      <c r="S249" s="5"/>
       <c r="T249" s="4"/>
       <c r="U249" s="5">
         <v>87</v>
@@ -33481,7 +33469,7 @@
       <c r="R250" s="6">
         <v>99.35652520693365</v>
       </c>
-      <c r="S250" s="7"/>
+      <c r="S250" s="5"/>
       <c r="T250" s="4"/>
       <c r="U250" s="5">
         <v>88</v>
@@ -33602,7 +33590,7 @@
       <c r="R251" s="6">
         <v>99.5178802930459</v>
       </c>
-      <c r="S251" s="7"/>
+      <c r="S251" s="5"/>
       <c r="T251" s="4"/>
       <c r="U251" s="5">
         <v>89</v>
@@ -33723,7 +33711,7 @@
       <c r="R252" s="6">
         <v>99.05860931064221</v>
       </c>
-      <c r="S252" s="7"/>
+      <c r="S252" s="5"/>
       <c r="T252" s="4"/>
       <c r="U252" s="5">
         <v>90</v>
@@ -33844,7 +33832,7 @@
       <c r="R253" s="6">
         <v>99.54875981232848</v>
       </c>
-      <c r="S253" s="7"/>
+      <c r="S253" s="5"/>
       <c r="T253" s="4"/>
       <c r="U253" s="5">
         <v>91</v>
@@ -33965,7 +33953,7 @@
       <c r="R254" s="6">
         <v>99.79210934468573</v>
       </c>
-      <c r="S254" s="7"/>
+      <c r="S254" s="5"/>
       <c r="T254" s="4"/>
       <c r="U254" s="5">
         <v>92</v>
@@ -34086,7 +34074,7 @@
       <c r="R255" s="6">
         <v>99.96392726612359</v>
       </c>
-      <c r="S255" s="7"/>
+      <c r="S255" s="5"/>
       <c r="T255" s="4"/>
       <c r="U255" s="5">
         <v>93</v>
@@ -34207,7 +34195,7 @@
       <c r="R256" s="6">
         <v>99.53704210663976</v>
       </c>
-      <c r="S256" s="7"/>
+      <c r="S256" s="5"/>
       <c r="T256" s="4"/>
       <c r="U256" s="5">
         <v>94</v>
@@ -34328,7 +34316,7 @@
       <c r="R257" s="6">
         <v>96.16285618092105</v>
       </c>
-      <c r="S257" s="7"/>
+      <c r="S257" s="5"/>
       <c r="T257" s="4"/>
       <c r="U257" s="5">
         <v>127</v>
@@ -34449,7 +34437,7 @@
       <c r="R258" s="6">
         <v>96.51042472401166</v>
       </c>
-      <c r="S258" s="7"/>
+      <c r="S258" s="5"/>
       <c r="T258" s="4"/>
       <c r="U258" s="5">
         <v>121</v>
@@ -34570,7 +34558,7 @@
       <c r="R259" s="6">
         <v>97.23743699377289</v>
       </c>
-      <c r="S259" s="7"/>
+      <c r="S259" s="5"/>
       <c r="T259" s="4"/>
       <c r="U259" s="5">
         <v>132</v>
@@ -34691,7 +34679,7 @@
       <c r="R260" s="6">
         <v>97.62015995209174</v>
       </c>
-      <c r="S260" s="7"/>
+      <c r="S260" s="5"/>
       <c r="T260" s="4"/>
       <c r="U260" s="5">
         <v>133</v>
@@ -34812,7 +34800,7 @@
       <c r="R261" s="6">
         <v>97.15070139521464</v>
       </c>
-      <c r="S261" s="7"/>
+      <c r="S261" s="5"/>
       <c r="T261" s="4"/>
       <c r="U261" s="5">
         <v>134</v>
@@ -34933,7 +34921,7 @@
       <c r="R262" s="6">
         <v>97.33026475842993</v>
       </c>
-      <c r="S262" s="7"/>
+      <c r="S262" s="5"/>
       <c r="T262" s="4"/>
       <c r="U262" s="5">
         <v>135</v>
@@ -35054,7 +35042,7 @@
       <c r="R263" s="6">
         <v>96.68890687220589</v>
       </c>
-      <c r="S263" s="7"/>
+      <c r="S263" s="5"/>
       <c r="T263" s="4"/>
       <c r="U263" s="5">
         <v>114</v>
@@ -35175,7 +35163,7 @@
       <c r="R264" s="6">
         <v>96.59307974978952</v>
       </c>
-      <c r="S264" s="7"/>
+      <c r="S264" s="5"/>
       <c r="T264" s="4"/>
       <c r="U264" s="5">
         <v>116</v>
@@ -35296,7 +35284,7 @@
       <c r="R265" s="6">
         <v>96.7391067372905</v>
       </c>
-      <c r="S265" s="7"/>
+      <c r="S265" s="5"/>
       <c r="T265" s="4"/>
       <c r="U265" s="5">
         <v>109</v>
@@ -35417,7 +35405,7 @@
       <c r="R266" s="6">
         <v>96.82008340455374</v>
       </c>
-      <c r="S266" s="7"/>
+      <c r="S266" s="5"/>
       <c r="T266" s="4"/>
       <c r="U266" s="5">
         <v>110</v>
@@ -35538,7 +35526,7 @@
       <c r="R267" s="6">
         <v>96.96317471336141</v>
       </c>
-      <c r="S267" s="7"/>
+      <c r="S267" s="5"/>
       <c r="T267" s="4"/>
       <c r="U267" s="5">
         <v>111</v>
@@ -35659,7 +35647,7 @@
       <c r="R268" s="6">
         <v>96.78526908649418</v>
       </c>
-      <c r="S268" s="7"/>
+      <c r="S268" s="5"/>
       <c r="T268" s="4"/>
       <c r="U268" s="5">
         <v>112</v>
@@ -35780,7 +35768,7 @@
       <c r="R269" s="6">
         <v>96.47103481426147</v>
       </c>
-      <c r="S269" s="7"/>
+      <c r="S269" s="5"/>
       <c r="T269" s="4"/>
       <c r="U269" s="5">
         <v>129</v>
@@ -35901,7 +35889,7 @@
       <c r="R270" s="6">
         <v>96.83815718986638</v>
       </c>
-      <c r="S270" s="7"/>
+      <c r="S270" s="5"/>
       <c r="T270" s="4"/>
       <c r="U270" s="5">
         <v>130</v>
@@ -36022,7 +36010,7 @@
       <c r="R271" s="6">
         <v>96.2636283621303</v>
       </c>
-      <c r="S271" s="7"/>
+      <c r="S271" s="5"/>
       <c r="T271" s="4"/>
       <c r="U271" s="5">
         <v>131</v>
@@ -36143,7 +36131,7 @@
       <c r="R272" s="6">
         <v>97.76826762044895</v>
       </c>
-      <c r="S272" s="7"/>
+      <c r="S272" s="5"/>
       <c r="T272" s="4"/>
       <c r="U272" s="5">
         <v>105</v>
@@ -36264,7 +36252,7 @@
       <c r="R273" s="6">
         <v>97.91469196694814</v>
       </c>
-      <c r="S273" s="7"/>
+      <c r="S273" s="5"/>
       <c r="T273" s="4"/>
       <c r="U273" s="5">
         <v>106</v>
@@ -36385,7 +36373,7 @@
       <c r="R274" s="6">
         <v>97.9482444687081</v>
       </c>
-      <c r="S274" s="7"/>
+      <c r="S274" s="5"/>
       <c r="T274" s="4"/>
       <c r="U274" s="5">
         <v>107</v>
@@ -36506,7 +36494,7 @@
       <c r="R275" s="6">
         <v>97.71272947401502</v>
       </c>
-      <c r="S275" s="7"/>
+      <c r="S275" s="5"/>
       <c r="T275" s="4"/>
       <c r="U275" s="5">
         <v>108</v>
@@ -36627,7 +36615,7 @@
       <c r="R276" s="6">
         <v>98.72028841554368</v>
       </c>
-      <c r="S276" s="7"/>
+      <c r="S276" s="5"/>
       <c r="T276" s="4"/>
       <c r="U276" s="5">
         <v>101</v>
@@ -36748,7 +36736,7 @@
       <c r="R277" s="6">
         <v>98.54725095883184</v>
       </c>
-      <c r="S277" s="7"/>
+      <c r="S277" s="5"/>
       <c r="T277" s="4"/>
       <c r="U277" s="5">
         <v>102</v>
@@ -36869,7 +36857,7 @@
       <c r="R278" s="6">
         <v>98.34460705279476</v>
       </c>
-      <c r="S278" s="7"/>
+      <c r="S278" s="5"/>
       <c r="T278" s="4"/>
       <c r="U278" s="5">
         <v>103</v>
@@ -36990,7 +36978,7 @@
       <c r="R279" s="6">
         <v>98.7939310940506</v>
       </c>
-      <c r="S279" s="7"/>
+      <c r="S279" s="5"/>
       <c r="T279" s="4"/>
       <c r="U279" s="5">
         <v>96</v>
@@ -37111,7 +37099,7 @@
       <c r="R280" s="6">
         <v>98.75612178993151</v>
       </c>
-      <c r="S280" s="7"/>
+      <c r="S280" s="5"/>
       <c r="T280" s="4"/>
       <c r="U280" s="5">
         <v>97</v>
@@ -37232,7 +37220,7 @@
       <c r="R281" s="6">
         <v>99.14795668009698</v>
       </c>
-      <c r="S281" s="7"/>
+      <c r="S281" s="5"/>
       <c r="T281" s="4"/>
       <c r="U281" s="5">
         <v>98</v>
@@ -37353,7 +37341,7 @@
       <c r="R282" s="6">
         <v>99.16352132334718</v>
       </c>
-      <c r="S282" s="7"/>
+      <c r="S282" s="5"/>
       <c r="T282" s="4"/>
       <c r="U282" s="5">
         <v>99</v>
@@ -37474,7 +37462,7 @@
       <c r="R283" s="6">
         <v>98.96582713188799</v>
       </c>
-      <c r="S283" s="7"/>
+      <c r="S283" s="5"/>
       <c r="T283" s="4"/>
       <c r="U283" s="5">
         <v>100</v>
@@ -37595,7 +37583,7 @@
       <c r="R284" s="6">
         <v>98.43335265813418</v>
       </c>
-      <c r="S284" s="7"/>
+      <c r="S284" s="5"/>
       <c r="T284" s="4"/>
       <c r="U284" s="5">
         <v>90</v>
@@ -37716,7 +37704,7 @@
       <c r="R285" s="6">
         <v>98.82372026743404</v>
       </c>
-      <c r="S285" s="7"/>
+      <c r="S285" s="5"/>
       <c r="T285" s="4"/>
       <c r="U285" s="5">
         <v>91</v>
@@ -37837,7 +37825,7 @@
       <c r="R286" s="6">
         <v>98.86950217884815</v>
       </c>
-      <c r="S286" s="7"/>
+      <c r="S286" s="5"/>
       <c r="T286" s="4"/>
       <c r="U286" s="5">
         <v>92</v>
@@ -37958,7 +37946,7 @@
       <c r="R287" s="6">
         <v>99.04250944371718</v>
       </c>
-      <c r="S287" s="7"/>
+      <c r="S287" s="5"/>
       <c r="T287" s="4"/>
       <c r="U287" s="5">
         <v>93</v>
@@ -38079,7 +38067,7 @@
       <c r="R288" s="6">
         <v>98.97130058077761</v>
       </c>
-      <c r="S288" s="7"/>
+      <c r="S288" s="5"/>
       <c r="T288" s="4"/>
       <c r="U288" s="5">
         <v>94</v>
@@ -38200,7 +38188,7 @@
       <c r="R289" s="6">
         <v>98.38800731661198</v>
       </c>
-      <c r="S289" s="7"/>
+      <c r="S289" s="5"/>
       <c r="T289" s="4"/>
       <c r="U289" s="5">
         <v>95</v>
@@ -38321,7 +38309,7 @@
       <c r="R290" s="6">
         <v>98.41334158910949</v>
       </c>
-      <c r="S290" s="7"/>
+      <c r="S290" s="5"/>
       <c r="T290" s="4"/>
       <c r="U290" s="5">
         <v>87</v>
@@ -38442,7 +38430,7 @@
       <c r="R291" s="6">
         <v>98.34119987537268</v>
       </c>
-      <c r="S291" s="7"/>
+      <c r="S291" s="5"/>
       <c r="T291" s="4"/>
       <c r="U291" s="5">
         <v>88</v>
@@ -38563,7 +38551,7 @@
       <c r="R292" s="6">
         <v>98.60595678144084</v>
       </c>
-      <c r="S292" s="7"/>
+      <c r="S292" s="5"/>
       <c r="T292" s="4"/>
       <c r="U292" s="5">
         <v>89</v>
@@ -38684,7 +38672,7 @@
       <c r="R293" s="6">
         <v>98.36245364985187</v>
       </c>
-      <c r="S293" s="7"/>
+      <c r="S293" s="5"/>
       <c r="T293" s="4"/>
       <c r="U293" s="5">
         <v>43</v>
@@ -38805,7 +38793,7 @@
       <c r="R294" s="6">
         <v>99.15838517082754</v>
       </c>
-      <c r="S294" s="7"/>
+      <c r="S294" s="5"/>
       <c r="T294" s="4"/>
       <c r="U294" s="5">
         <v>44</v>
@@ -38926,7 +38914,7 @@
       <c r="R295" s="6">
         <v>98.67392289291568</v>
       </c>
-      <c r="S295" s="7"/>
+      <c r="S295" s="5"/>
       <c r="T295" s="4"/>
       <c r="U295" s="5">
         <v>45</v>
@@ -39047,7 +39035,7 @@
       <c r="R296" s="6">
         <v>98.27225360858931</v>
       </c>
-      <c r="S296" s="7"/>
+      <c r="S296" s="5"/>
       <c r="T296" s="4"/>
       <c r="U296" s="5">
         <v>46</v>
@@ -39168,7 +39156,7 @@
       <c r="R297" s="6">
         <v>98.63396358747562</v>
       </c>
-      <c r="S297" s="7"/>
+      <c r="S297" s="5"/>
       <c r="T297" s="4"/>
       <c r="U297" s="5">
         <v>47</v>
@@ -39289,7 +39277,7 @@
       <c r="R298" s="6">
         <v>98.58018993144391</v>
       </c>
-      <c r="S298" s="7"/>
+      <c r="S298" s="5"/>
       <c r="T298" s="4"/>
       <c r="U298" s="5">
         <v>23</v>
@@ -39410,7 +39398,7 @@
       <c r="R299" s="6">
         <v>98.88571101044029</v>
       </c>
-      <c r="S299" s="7"/>
+      <c r="S299" s="5"/>
       <c r="T299" s="4"/>
       <c r="U299" s="5">
         <v>24</v>
@@ -39531,7 +39519,7 @@
       <c r="R300" s="6">
         <v>98.68393805179089</v>
       </c>
-      <c r="S300" s="7"/>
+      <c r="S300" s="5"/>
       <c r="T300" s="4"/>
       <c r="U300" s="5">
         <v>25</v>
@@ -39652,7 +39640,7 @@
       <c r="R301" s="6">
         <v>98.35122707314717</v>
       </c>
-      <c r="S301" s="7"/>
+      <c r="S301" s="5"/>
       <c r="T301" s="4"/>
       <c r="U301" s="5">
         <v>26</v>
@@ -39773,7 +39761,7 @@
       <c r="R302" s="6">
         <v>98.11530856190585</v>
       </c>
-      <c r="S302" s="7"/>
+      <c r="S302" s="5"/>
       <c r="T302" s="4"/>
       <c r="U302" s="5">
         <v>27</v>
@@ -39894,7 +39882,7 @@
       <c r="R303" s="6">
         <v>97.98873228978452</v>
       </c>
-      <c r="S303" s="7"/>
+      <c r="S303" s="5"/>
       <c r="T303" s="4"/>
       <c r="U303" s="5">
         <v>18</v>
@@ -40015,7 +40003,7 @@
       <c r="R304" s="6">
         <v>98.32036435425522</v>
       </c>
-      <c r="S304" s="7"/>
+      <c r="S304" s="5"/>
       <c r="T304" s="4"/>
       <c r="U304" s="5">
         <v>19</v>
@@ -40136,7 +40124,7 @@
       <c r="R305" s="6">
         <v>98.05975833796782</v>
       </c>
-      <c r="S305" s="7"/>
+      <c r="S305" s="5"/>
       <c r="T305" s="4"/>
       <c r="U305" s="5">
         <v>20</v>
@@ -40257,7 +40245,7 @@
       <c r="R306" s="6">
         <v>98.20638734454523</v>
       </c>
-      <c r="S306" s="7"/>
+      <c r="S306" s="5"/>
       <c r="T306" s="4"/>
       <c r="U306" s="5">
         <v>21</v>
@@ -40378,7 +40366,7 @@
       <c r="R307" s="6">
         <v>98.42153697668574</v>
       </c>
-      <c r="S307" s="7"/>
+      <c r="S307" s="5"/>
       <c r="T307" s="4"/>
       <c r="U307" s="5">
         <v>22</v>
@@ -40499,7 +40487,7 @@
       <c r="R308" s="6">
         <v>96.71699369257105</v>
       </c>
-      <c r="S308" s="7"/>
+      <c r="S308" s="5"/>
       <c r="T308" s="4"/>
       <c r="U308" s="5">
         <v>14</v>
@@ -40620,7 +40608,7 @@
       <c r="R309" s="6">
         <v>96.8389094680641</v>
       </c>
-      <c r="S309" s="7"/>
+      <c r="S309" s="5"/>
       <c r="T309" s="4"/>
       <c r="U309" s="5">
         <v>15</v>
@@ -40741,7 +40729,7 @@
       <c r="R310" s="6">
         <v>96.91000696234185</v>
       </c>
-      <c r="S310" s="7"/>
+      <c r="S310" s="5"/>
       <c r="T310" s="4"/>
       <c r="U310" s="5">
         <v>16</v>
@@ -40862,7 +40850,7 @@
       <c r="R311" s="6">
         <v>96.38566386609311</v>
       </c>
-      <c r="S311" s="7"/>
+      <c r="S311" s="5"/>
       <c r="T311" s="4"/>
       <c r="U311" s="5">
         <v>17</v>
@@ -40983,7 +40971,7 @@
       <c r="R312" s="6">
         <v>96.35566717435096</v>
       </c>
-      <c r="S312" s="7"/>
+      <c r="S312" s="5"/>
       <c r="T312" s="4"/>
       <c r="U312" s="5">
         <v>10</v>
@@ -41104,7 +41092,7 @@
       <c r="R313" s="6">
         <v>96.58096240024061</v>
       </c>
-      <c r="S313" s="7"/>
+      <c r="S313" s="5"/>
       <c r="T313" s="4"/>
       <c r="U313" s="5">
         <v>11</v>
@@ -41225,7 +41213,7 @@
       <c r="R314" s="6">
         <v>96.31923405023065</v>
       </c>
-      <c r="S314" s="7"/>
+      <c r="S314" s="5"/>
       <c r="T314" s="4"/>
       <c r="U314" s="5">
         <v>12</v>
@@ -41346,7 +41334,7 @@
       <c r="R315" s="6">
         <v>99.0275728331925</v>
       </c>
-      <c r="S315" s="7"/>
+      <c r="S315" s="5"/>
       <c r="T315" s="4"/>
       <c r="U315" s="5">
         <v>74</v>
@@ -41467,7 +41455,7 @@
       <c r="R316" s="6">
         <v>98.91584027145906</v>
       </c>
-      <c r="S316" s="7"/>
+      <c r="S316" s="5"/>
       <c r="T316" s="4"/>
       <c r="U316" s="5">
         <v>75</v>
@@ -41588,7 +41576,7 @@
       <c r="R317" s="6">
         <v>98.56356170064278</v>
       </c>
-      <c r="S317" s="7"/>
+      <c r="S317" s="5"/>
       <c r="T317" s="4"/>
       <c r="U317" s="5">
         <v>76</v>
@@ -41709,7 +41697,7 @@
       <c r="R318" s="6">
         <v>98.5023016836405</v>
       </c>
-      <c r="S318" s="7"/>
+      <c r="S318" s="5"/>
       <c r="T318" s="4"/>
       <c r="U318" s="5">
         <v>77</v>
@@ -41830,7 +41818,7 @@
       <c r="R319" s="6">
         <v>99.11179760048807</v>
       </c>
-      <c r="S319" s="7"/>
+      <c r="S319" s="5"/>
       <c r="T319" s="4"/>
       <c r="U319" s="5">
         <v>78</v>
@@ -41951,7 +41939,7 @@
       <c r="R320" s="6">
         <v>98.56368971647079</v>
       </c>
-      <c r="S320" s="7"/>
+      <c r="S320" s="5"/>
       <c r="T320" s="4"/>
       <c r="U320" s="5">
         <v>79</v>
@@ -42072,7 +42060,7 @@
       <c r="R321" s="6">
         <v>98.85322455645232</v>
       </c>
-      <c r="S321" s="7"/>
+      <c r="S321" s="5"/>
       <c r="T321" s="4"/>
       <c r="U321" s="5">
         <v>80</v>
@@ -42193,7 +42181,7 @@
       <c r="R322" s="6">
         <v>98.12554648905449</v>
       </c>
-      <c r="S322" s="7"/>
+      <c r="S322" s="5"/>
       <c r="T322" s="4"/>
       <c r="U322" s="5">
         <v>81</v>
@@ -42314,7 +42302,7 @@
       <c r="R323" s="6">
         <v>98.11375907050989</v>
       </c>
-      <c r="S323" s="7"/>
+      <c r="S323" s="5"/>
       <c r="T323" s="4"/>
       <c r="U323" s="5">
         <v>82</v>
@@ -42435,7 +42423,7 @@
       <c r="R324" s="6">
         <v>98.528578803063</v>
       </c>
-      <c r="S324" s="7"/>
+      <c r="S324" s="5"/>
       <c r="T324" s="4"/>
       <c r="U324" s="5">
         <v>67</v>
@@ -42556,7 +42544,7 @@
       <c r="R325" s="6">
         <v>98.38896023382942</v>
       </c>
-      <c r="S325" s="7"/>
+      <c r="S325" s="5"/>
       <c r="T325" s="4"/>
       <c r="U325" s="5">
         <v>68</v>
@@ -42677,7 +42665,7 @@
       <c r="R326" s="6">
         <v>98.89192604503249</v>
       </c>
-      <c r="S326" s="7"/>
+      <c r="S326" s="5"/>
       <c r="T326" s="4"/>
       <c r="U326" s="5">
         <v>69</v>
@@ -42798,7 +42786,7 @@
       <c r="R327" s="6">
         <v>98.18552683127967</v>
       </c>
-      <c r="S327" s="7"/>
+      <c r="S327" s="5"/>
       <c r="T327" s="4"/>
       <c r="U327" s="5">
         <v>70</v>
@@ -42919,7 +42907,7 @@
       <c r="R328" s="6">
         <v>98.45560311894485</v>
       </c>
-      <c r="S328" s="7"/>
+      <c r="S328" s="5"/>
       <c r="T328" s="4"/>
       <c r="U328" s="5">
         <v>71</v>
@@ -43040,7 +43028,7 @@
       <c r="R329" s="6">
         <v>99.39391691056339</v>
       </c>
-      <c r="S329" s="7"/>
+      <c r="S329" s="5"/>
       <c r="T329" s="4"/>
       <c r="U329" s="5">
         <v>72</v>
@@ -43161,7 +43149,7 @@
       <c r="R330" s="6">
         <v>98.55017704811215</v>
       </c>
-      <c r="S330" s="7"/>
+      <c r="S330" s="5"/>
       <c r="T330" s="4"/>
       <c r="U330" s="5">
         <v>73</v>
@@ -43282,7 +43270,7 @@
       <c r="R331" s="6">
         <v>98.62123901583398</v>
       </c>
-      <c r="S331" s="7"/>
+      <c r="S331" s="5"/>
       <c r="T331" s="4"/>
       <c r="U331" s="5">
         <v>38</v>
@@ -43403,7 +43391,7 @@
       <c r="R332" s="6">
         <v>98.8004138330336</v>
       </c>
-      <c r="S332" s="7"/>
+      <c r="S332" s="5"/>
       <c r="T332" s="4"/>
       <c r="U332" s="5">
         <v>39</v>
@@ -43524,7 +43512,7 @@
       <c r="R333" s="6">
         <v>98.70815728946717</v>
       </c>
-      <c r="S333" s="7"/>
+      <c r="S333" s="5"/>
       <c r="T333" s="4"/>
       <c r="U333" s="5">
         <v>40</v>
@@ -43645,7 +43633,7 @@
       <c r="R334" s="6">
         <v>98.43424258303199</v>
       </c>
-      <c r="S334" s="7"/>
+      <c r="S334" s="5"/>
       <c r="T334" s="4"/>
       <c r="U334" s="5">
         <v>41</v>
@@ -43766,7 +43754,7 @@
       <c r="R335" s="6">
         <v>98.93733888066913</v>
       </c>
-      <c r="S335" s="7"/>
+      <c r="S335" s="5"/>
       <c r="T335" s="4"/>
       <c r="U335" s="5">
         <v>42</v>
@@ -43887,7 +43875,7 @@
       <c r="R336" s="6">
         <v>98.92382195679778</v>
       </c>
-      <c r="S336" s="7"/>
+      <c r="S336" s="5"/>
       <c r="T336" s="4"/>
       <c r="U336" s="5">
         <v>33</v>
@@ -44008,7 +43996,7 @@
       <c r="R337" s="6">
         <v>98.90268487093014</v>
       </c>
-      <c r="S337" s="7"/>
+      <c r="S337" s="5"/>
       <c r="T337" s="4"/>
       <c r="U337" s="5">
         <v>34</v>
@@ -44129,7 +44117,7 @@
       <c r="R338" s="6">
         <v>98.98311797575248</v>
       </c>
-      <c r="S338" s="7"/>
+      <c r="S338" s="5"/>
       <c r="T338" s="4"/>
       <c r="U338" s="5">
         <v>36</v>
@@ -44250,7 +44238,7 @@
       <c r="R339" s="6">
         <v>98.35915832313994</v>
       </c>
-      <c r="S339" s="7"/>
+      <c r="S339" s="5"/>
       <c r="T339" s="4"/>
       <c r="U339" s="5">
         <v>37</v>
@@ -44371,7 +44359,7 @@
       <c r="R340" s="6">
         <v>98.86931946521567</v>
       </c>
-      <c r="S340" s="7"/>
+      <c r="S340" s="5"/>
       <c r="T340" s="4"/>
       <c r="U340" s="5">
         <v>28</v>
@@ -44492,7 +44480,7 @@
       <c r="R341" s="6">
         <v>98.81645711733377</v>
       </c>
-      <c r="S341" s="7"/>
+      <c r="S341" s="5"/>
       <c r="T341" s="4"/>
       <c r="U341" s="5">
         <v>29</v>
@@ -44613,7 +44601,7 @@
       <c r="R342" s="6">
         <v>98.79587795538833</v>
       </c>
-      <c r="S342" s="7"/>
+      <c r="S342" s="5"/>
       <c r="T342" s="4"/>
       <c r="U342" s="5">
         <v>30</v>
@@ -44734,7 +44722,7 @@
       <c r="R343" s="6">
         <v>99.2040815428306</v>
       </c>
-      <c r="S343" s="7"/>
+      <c r="S343" s="5"/>
       <c r="T343" s="4"/>
       <c r="U343" s="5">
         <v>31</v>
@@ -44855,7 +44843,7 @@
       <c r="R344" s="6">
         <v>99.9914097997949</v>
       </c>
-      <c r="S344" s="7"/>
+      <c r="S344" s="5"/>
       <c r="T344" s="4"/>
       <c r="U344" s="5">
         <v>32</v>

</xml_diff>